<commit_message>
feat: update Time Reward config
更新在线奖励表
</commit_message>
<xml_diff>
--- a/pet-simulator/Excel/TimeReward_在线奖励表.xlsx
+++ b/pet-simulator/Excel/TimeReward_在线奖励表.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\P12GPark\Project\Edit\DragonVerse\pet-simulator\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0001B7F7-9065-4510-BAF4-D95884C8C495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05356333-2E82-4505-9ED7-69A53F6066DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>int</t>
   </si>
@@ -119,43 +119,44 @@
     <t>礼包12</t>
   </si>
   <si>
-    <t>0|10000|0|0</t>
+    <t>15000|1000|0|0</t>
+  </si>
+  <si>
+    <t>20000|1500|0|0</t>
+  </si>
+  <si>
+    <t>30000|2000|0|0</t>
+  </si>
+  <si>
+    <t>40000|2500|0|0</t>
+  </si>
+  <si>
+    <t>50000|3000|0|0</t>
+  </si>
+  <si>
+    <t>50000|4000|0|0</t>
+  </si>
+  <si>
+    <t>50000|5000|0|0</t>
+  </si>
+  <si>
+    <t>500|100|0|0</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>100|1000|0|0</t>
+    <t>3000|300|0|0</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>0|2000|0|0</t>
+    <t>10000|600|0|0</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>0|3000|0|0</t>
+    <t>6000|500|0|0</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>0|4000|0|0</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>50000|0|0|0</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>0|6000|0|0</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>0|7000|0|0</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>0|8000|0|0</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>0|9000|0|0</t>
+    <t>1000|200|0|0</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -558,7 +559,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.28515625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -649,13 +650,13 @@
         <v>17</v>
       </c>
       <c r="C5" s="2">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="D5" s="1">
         <v>174803</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F5" s="5">
         <v>0</v>
@@ -672,13 +673,13 @@
         <v>19</v>
       </c>
       <c r="C6" s="2">
-        <v>480</v>
+        <v>600</v>
       </c>
       <c r="D6" s="1">
         <v>174803</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F6" s="5">
         <v>0</v>
@@ -701,7 +702,7 @@
         <v>174824</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F7" s="5">
         <v>0</v>
@@ -718,13 +719,13 @@
         <v>22</v>
       </c>
       <c r="C8" s="2">
-        <v>1200</v>
+        <v>1800</v>
       </c>
       <c r="D8" s="1">
         <v>174824</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
@@ -741,13 +742,13 @@
         <v>23</v>
       </c>
       <c r="C9" s="2">
-        <v>1800</v>
+        <v>3600</v>
       </c>
       <c r="D9" s="1">
         <v>174824</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F9" s="5">
         <v>0</v>
@@ -764,13 +765,13 @@
         <v>24</v>
       </c>
       <c r="C10" s="2">
-        <v>2400</v>
+        <v>7200</v>
       </c>
       <c r="D10" s="1">
         <v>174837</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F10" s="5">
         <v>0</v>
@@ -787,13 +788,13 @@
         <v>25</v>
       </c>
       <c r="C11" s="2">
-        <v>3000</v>
+        <v>10800</v>
       </c>
       <c r="D11" s="1">
         <v>174837</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F11" s="5">
         <v>0</v>
@@ -810,13 +811,13 @@
         <v>26</v>
       </c>
       <c r="C12" s="1">
-        <v>3600</v>
+        <v>18000</v>
       </c>
       <c r="D12" s="1">
         <v>174837</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F12" s="5">
         <v>0</v>
@@ -833,13 +834,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="1">
-        <v>4500</v>
+        <v>28800</v>
       </c>
       <c r="D13" s="1">
         <v>174804</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F13" s="5">
         <v>0</v>
@@ -856,13 +857,13 @@
         <v>28</v>
       </c>
       <c r="C14" s="1">
-        <v>5400</v>
+        <v>43200</v>
       </c>
       <c r="D14" s="1">
         <v>174804</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F14" s="5">
         <v>0</v>
@@ -879,13 +880,13 @@
         <v>29</v>
       </c>
       <c r="C15" s="1">
-        <v>7200</v>
+        <v>61200</v>
       </c>
       <c r="D15" s="1">
         <v>174804</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F15" s="5">
         <v>0</v>
@@ -902,13 +903,13 @@
         <v>30</v>
       </c>
       <c r="C16" s="1">
-        <v>10800</v>
+        <v>86400</v>
       </c>
       <c r="D16" s="1">
         <v>174804</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F16" s="5">
         <v>0</v>
@@ -926,13 +927,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <pixelatorList sheetStid="1"/>
-  <pixelatorList sheetStid="2"/>
-</pixelators>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <woProps xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <woSheetsProps>
     <woSheetProps sheetStid="1" interlineOnOff="0" interlineColor="0" isDbSheet="0" isDashBoardSheet="0">
@@ -945,8 +939,15 @@
 </woProps>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <pixelatorList sheetStid="1"/>
+  <pixelatorList sheetStid="2"/>
+</pixelators>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C82605-B75B-4693-9329-32AAD527C692}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
@@ -955,7 +956,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C82605-B75B-4693-9329-32AAD527C692}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>

</xml_diff>